<commit_message>
[ENH] budget report unit, add column
</commit_message>
<xml_diff>
--- a/pabi_budget_report/xlsx_template/xlsx_report_budget_plan_unit_analysis.xlsx
+++ b/pabi_budget_report/xlsx_template/xlsx_report_budget_plan_unit_analysis.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t xml:space="preserve">Financial Year</t>
   </si>
@@ -82,7 +82,10 @@
     <t xml:space="preserve">Mission</t>
   </si>
   <si>
-    <t xml:space="preserve">Activity Group</t>
+    <t xml:space="preserve">AG Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AG Name</t>
   </si>
   <si>
     <t xml:space="preserve">Job Order Code</t>
@@ -149,6 +152,9 @@
   </si>
   <si>
     <t xml:space="preserve">Planned Amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State</t>
   </si>
 </sst>
 </file>
@@ -299,67 +305,67 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AL11"/>
+  <dimension ref="A1:AN11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AI1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AP11" activeCellId="0" sqref="AP11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="1" style="0" width="24.95"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="39" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="1" style="0" width="24.95"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="40" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -398,8 +404,9 @@
       <c r="AJ9" s="3"/>
       <c r="AK9" s="3"/>
       <c r="AL9" s="3"/>
-    </row>
-    <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AM9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -514,8 +521,14 @@
       <c r="AL10" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AM10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AN10" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>

</xml_diff>